<commit_message>
After asynch video upload to repo
</commit_message>
<xml_diff>
--- a/potterydata.xlsx
+++ b/potterydata.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bivinsadler/Box/BoxDept_MSDS - course files/MSDS 6306 Doing Data Science/NEW DDS/UNIT 6/LIve Session/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tgarn\OneDrive\Desktop\SMU - MS Data Science\Courses\GitHub\DS_6306_weekly_assignments\Week_6\Todd_Garner_DS6306_Week6_FLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD8332B4-8443-1946-806F-4580EB5A5F9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B42AFF-ED81-4FF8-B077-51CE8ECEE7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="13300" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -433,9 +431,9 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -455,7 +453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>14.4</v>
       </c>
@@ -475,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13.8</v>
       </c>
@@ -495,7 +493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14.6</v>
       </c>
@@ -515,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11.5</v>
       </c>
@@ -535,7 +533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13.8</v>
       </c>
@@ -555,7 +553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10.9</v>
       </c>
@@ -575,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10.1</v>
       </c>
@@ -595,7 +593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11.6</v>
       </c>
@@ -615,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11.1</v>
       </c>
@@ -635,7 +633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13.4</v>
       </c>
@@ -655,7 +653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12.4</v>
       </c>
@@ -675,7 +673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13.1</v>
       </c>
@@ -695,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12.7</v>
       </c>
@@ -715,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12.5</v>
       </c>
@@ -735,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11.8</v>
       </c>
@@ -755,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11.6</v>
       </c>
@@ -775,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18.3</v>
       </c>
@@ -795,7 +793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15.8</v>
       </c>
@@ -815,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -835,7 +833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -855,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20.8</v>
       </c>
@@ -875,7 +873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17.7</v>
       </c>
@@ -895,7 +893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18.3</v>
       </c>
@@ -915,7 +913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16.7</v>
       </c>
@@ -935,7 +933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>14.8</v>
       </c>
@@ -955,7 +953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19.100000000000001</v>
       </c>
@@ -978,28 +976,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>